<commit_message>
add payload for update event status
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC856093-CDD5-4AD2-990A-2C69EF20A9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BAFB0-AE6C-4478-B008-4D848D2C9EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3560,7 +3560,7 @@
   <dimension ref="A1:F691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13301,21 +13301,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13512,24 +13497,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13546,4 +13529,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update template for section import
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BAFB0-AE6C-4478-B008-4D848D2C9EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D82DD-9A80-4527-BE62-8ACC6998FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1052">
   <si>
     <t>property</t>
   </si>
@@ -3560,7 +3560,7 @@
   <dimension ref="A1:F691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3801,6 +3801,9 @@
       <c r="D13" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="E13" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -13301,6 +13304,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13497,22 +13515,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13529,21 +13549,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update format for import translation
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D82DD-9A80-4527-BE62-8ACC6998FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096D9CF-D431-4CCA-B548-59449DFD48A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataElements" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="1055">
   <si>
     <t>property</t>
   </si>
@@ -3187,6 +3187,15 @@
   </si>
   <si>
     <t>relationshipTypes</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>programStages</t>
   </si>
 </sst>
 </file>
@@ -3557,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
-  <dimension ref="A1:F691"/>
+  <dimension ref="A1:H691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3572,7 +3581,7 @@
     <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3591,8 +3600,11 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3611,8 +3623,14 @@
       <c r="F2" s="2" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -3632,7 +3650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3669,7 +3687,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3686,7 +3704,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3703,7 +3721,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -3720,7 +3738,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -3734,10 +3752,10 @@
         <v>358</v>
       </c>
       <c r="E9" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -3754,7 +3772,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -3771,7 +3789,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -3805,7 +3823,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -3819,7 +3837,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -3833,7 +3851,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -13304,18 +13322,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13516,18 +13534,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add pay load for update multiple events dataValues
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C839AC-99E8-480F-9F9D-09ACF34CBBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B987A7A-ECB9-44F6-95F4-307CF4C8EB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataElements!$D$1:$D$94</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="1067">
   <si>
     <t>property</t>
   </si>
@@ -3209,6 +3209,33 @@
   </si>
   <si>
     <t>fr</t>
+  </si>
+  <si>
+    <t>arabic</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Ukrainian (Ukraine)</t>
+  </si>
+  <si>
+    <t>uk_UA</t>
+  </si>
+  <si>
+    <t>dataSets</t>
+  </si>
+  <si>
+    <t>categoryCombos</t>
+  </si>
+  <si>
+    <t>optionSets</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>for trackedEntityAttributes remove form-name then translation work</t>
   </si>
 </sst>
 </file>
@@ -3581,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
   <dimension ref="A1:H691"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3657,7 +3684,7 @@
       <c r="D3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1042</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3683,11 +3710,17 @@
       <c r="D4" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>1043</v>
       </c>
       <c r="F4" t="s">
         <v>1044</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3706,6 +3739,12 @@
       <c r="E5" t="s">
         <v>1041</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -3805,7 +3844,7 @@
       <c r="D11" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -3873,6 +3912,9 @@
       <c r="D15" s="4" t="s">
         <v>364</v>
       </c>
+      <c r="E15" t="s">
+        <v>1062</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3887,8 +3929,11 @@
       <c r="D16" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -3901,8 +3946,11 @@
       <c r="D17" s="3" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -3916,7 +3964,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -3930,7 +3978,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -3943,8 +3991,14 @@
       <c r="D20" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -3958,7 +4012,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -3972,7 +4026,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -3986,7 +4040,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -4000,7 +4054,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -4014,7 +4068,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -4028,7 +4082,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -4042,7 +4096,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -4056,7 +4110,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -4070,7 +4124,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
@@ -4084,7 +4138,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -4098,7 +4152,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
@@ -13345,6 +13399,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13541,22 +13610,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13573,21 +13644,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add pay load for integration from one instance to other of event dataValue
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C839AC-99E8-480F-9F9D-09ACF34CBBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B987A7A-ECB9-44F6-95F4-307CF4C8EB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataElements!$D$1:$D$94</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="1067">
   <si>
     <t>property</t>
   </si>
@@ -3209,6 +3209,33 @@
   </si>
   <si>
     <t>fr</t>
+  </si>
+  <si>
+    <t>arabic</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Ukrainian (Ukraine)</t>
+  </si>
+  <si>
+    <t>uk_UA</t>
+  </si>
+  <si>
+    <t>dataSets</t>
+  </si>
+  <si>
+    <t>categoryCombos</t>
+  </si>
+  <si>
+    <t>optionSets</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>for trackedEntityAttributes remove form-name then translation work</t>
   </si>
 </sst>
 </file>
@@ -3581,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
   <dimension ref="A1:H691"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3657,7 +3684,7 @@
       <c r="D3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1042</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3683,11 +3710,17 @@
       <c r="D4" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>1043</v>
       </c>
       <c r="F4" t="s">
         <v>1044</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3706,6 +3739,12 @@
       <c r="E5" t="s">
         <v>1041</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -3805,7 +3844,7 @@
       <c r="D11" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -3873,6 +3912,9 @@
       <c r="D15" s="4" t="s">
         <v>364</v>
       </c>
+      <c r="E15" t="s">
+        <v>1062</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3887,8 +3929,11 @@
       <c r="D16" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -3901,8 +3946,11 @@
       <c r="D17" s="3" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -3916,7 +3964,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -3930,7 +3978,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -3943,8 +3991,14 @@
       <c r="D20" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -3958,7 +4012,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -3972,7 +4026,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -3986,7 +4040,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -4000,7 +4054,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -4014,7 +4068,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -4028,7 +4082,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -4042,7 +4096,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -4056,7 +4110,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -4070,7 +4124,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
@@ -4084,7 +4138,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -4098,7 +4152,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
@@ -13345,6 +13399,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13541,22 +13610,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13573,21 +13644,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update/add eventDataValue and enrollmentOrgUnit update payload
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6296DC25-1654-4314-BB35-9CD503DFF6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BD19B3-2E22-451C-B470-13095D8C9073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="1067">
   <si>
     <t>property</t>
   </si>
@@ -3608,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
   <dimension ref="A1:H691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3963,6 +3963,9 @@
       <c r="D18" s="3" t="s">
         <v>367</v>
       </c>
+      <c r="E18" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -13399,18 +13402,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13611,18 +13614,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add payload for update programindicator
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BD19B3-2E22-451C-B470-13095D8C9073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3E835-9063-4A9B-87BE-361BE20B7BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="1070">
   <si>
     <t>property</t>
   </si>
@@ -3236,6 +3236,15 @@
   </si>
   <si>
     <t>for trackedEntityAttributes remove form-name then translation work</t>
+  </si>
+  <si>
+    <t>programIndicators</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>vi</t>
   </si>
 </sst>
 </file>
@@ -3609,7 +3618,7 @@
   <dimension ref="A1:H691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3762,6 +3771,12 @@
       <c r="E6" t="s">
         <v>1045</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1069</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -4027,6 +4042,9 @@
       </c>
       <c r="D22" s="3" t="s">
         <v>371</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update format and add logic for calulate age based on dob and current-date
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3E835-9063-4A9B-87BE-361BE20B7BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B8E4B-BFF0-4FCF-902E-BD17A70E609B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3618,7 +3618,7 @@
   <dimension ref="A1:H691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13420,21 +13420,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13631,24 +13616,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13665,4 +13648,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add paylaod for post category without options
</commit_message>
<xml_diff>
--- a/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B8E4B-BFF0-4FCF-902E-BD17A70E609B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA72CEAB-BDB2-4FE3-9579-AE83BDE5D78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="1072">
   <si>
     <t>property</t>
   </si>
@@ -3245,6 +3245,12 @@
   </si>
   <si>
     <t>vi</t>
+  </si>
+  <si>
+    <t>Tetum</t>
+  </si>
+  <si>
+    <t>tet</t>
   </si>
 </sst>
 </file>
@@ -3618,7 +3624,7 @@
   <dimension ref="A1:H691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3794,6 +3800,12 @@
       <c r="E7" t="s">
         <v>1046</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1071</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -13420,6 +13432,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13616,12 +13634,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13632,6 +13644,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13650,15 +13671,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>

</xml_diff>